<commit_message>
Adding mapping models to result model
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS Sql Name Mapping.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS Sql Name Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robson/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Project/judo-tatami/judo-tatami-asm2rdbms/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,25 +24,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SqlName</t>
   </si>
   <si>
     <t>FullyQualifiedName</t>
+  </si>
+  <si>
+    <t>northwind.entities.City</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>northwind.entities.Territory#shipper</t>
+  </si>
+  <si>
+    <t>ID_SHIPPER</t>
+  </si>
+  <si>
+    <t>northwind.entities.Person#firstName</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -66,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -394,14 +420,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>